<commit_message>
Project Phase 1 checkpoint
</commit_message>
<xml_diff>
--- a/GradeTracker.xlsx
+++ b/GradeTracker.xlsx
@@ -1,22 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\git\CSC555\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AF33F0A-2847-4FDC-BD5A-DA0EDA97D81B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="135" windowWidth="19155" windowHeight="9780"/>
+    <workbookView xWindow="15" yWindow="15" windowWidth="28770" windowHeight="15570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Homeworks</t>
   </si>
@@ -43,12 +57,15 @@
   </si>
   <si>
     <t>Final Grade</t>
+  </si>
+  <si>
+    <t>hw5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -108,6 +125,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -155,7 +175,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -188,9 +208,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -223,6 +260,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -398,11 +452,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -470,52 +524,63 @@
       <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="1">
-        <v>100</v>
-      </c>
-      <c r="C5" s="3">
+      <c r="B5">
+        <v>100</v>
+      </c>
+      <c r="C5" s="2">
         <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B6">
-        <f>SUM(B2:B5)</f>
-        <v>400</v>
-      </c>
-      <c r="C6">
-        <f>SUM(C2:C5)</f>
-        <v>398</v>
-      </c>
-      <c r="D6">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1">
+        <v>100</v>
+      </c>
+      <c r="C6" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <f>SUM(B2:B6)</f>
+        <v>500</v>
+      </c>
+      <c r="C7">
+        <f>SUM(C2:C6)</f>
+        <v>498</v>
+      </c>
+      <c r="D7">
         <v>0.45</v>
       </c>
-      <c r="E6">
-        <f>(C6/B6)*D6</f>
-        <v>0.44774999999999998</v>
-      </c>
-      <c r="G6">
-        <f>SUM(G2:G5)</f>
+      <c r="E7">
+        <f>(C7/B7)*D7</f>
+        <v>0.44819999999999999</v>
+      </c>
+      <c r="G7">
+        <f>SUM(G2:G6)</f>
         <v>130</v>
       </c>
-      <c r="H6">
-        <f>SUM(H2:H5)</f>
+      <c r="H7">
+        <f>SUM(H2:H6)</f>
         <v>114</v>
       </c>
-      <c r="I6">
+      <c r="I7">
         <v>0.55000000000000004</v>
       </c>
-      <c r="J6">
-        <f>(H6/G6)*I6</f>
+      <c r="J7">
+        <f>(H7/G7)*I7</f>
         <v>0.48230769230769233</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>8</v>
       </c>
-      <c r="B10">
-        <f>E6+J6</f>
-        <v>0.93005769230769231</v>
+      <c r="B11">
+        <f>E7+J7</f>
+        <v>0.93050769230769226</v>
       </c>
     </row>
   </sheetData>
@@ -524,7 +589,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -536,7 +601,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
added assignment 3 grade
</commit_message>
<xml_diff>
--- a/GradeTracker.xlsx
+++ b/GradeTracker.xlsx
@@ -1,23 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21231"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\git\CSC555\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AF33F0A-2847-4FDC-BD5A-DA0EDA97D81B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="15" windowWidth="28770" windowHeight="15570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15" yWindow="15" windowWidth="28770" windowHeight="15570"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -30,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Homeworks</t>
   </si>
@@ -53,19 +47,22 @@
     <t>part2</t>
   </si>
   <si>
-    <t>hw4?</t>
-  </si>
-  <si>
     <t>Final Grade</t>
   </si>
   <si>
     <t>hw5</t>
+  </si>
+  <si>
+    <t>hw4</t>
+  </si>
+  <si>
+    <t>Estimated</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -110,11 +107,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -175,7 +173,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -208,26 +206,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -260,23 +241,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -452,24 +416,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="11" max="11" width="10.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="F1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -489,7 +459,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -506,34 +476,34 @@
         <v>100</v>
       </c>
       <c r="H3" s="3">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4">
         <v>100</v>
       </c>
-      <c r="C4" s="2">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C4" s="4">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B5">
         <v>100</v>
       </c>
       <c r="C5" s="2">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" s="1">
         <v>100</v>
@@ -542,45 +512,45 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7">
         <f>SUM(B2:B6)</f>
         <v>500</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="2">
         <f>SUM(C2:C6)</f>
-        <v>498</v>
+        <v>488</v>
       </c>
       <c r="D7">
         <v>0.45</v>
       </c>
       <c r="E7">
         <f>(C7/B7)*D7</f>
-        <v>0.44819999999999999</v>
+        <v>0.43919999999999998</v>
       </c>
       <c r="G7">
         <f>SUM(G2:G6)</f>
         <v>130</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="2">
         <f>SUM(H2:H6)</f>
-        <v>114</v>
+        <v>130</v>
       </c>
       <c r="I7">
         <v>0.55000000000000004</v>
       </c>
       <c r="J7">
         <f>(H7/G7)*I7</f>
-        <v>0.48230769230769233</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11">
+        <v>7</v>
+      </c>
+      <c r="B11" s="2">
         <f>E7+J7</f>
-        <v>0.93050769230769226</v>
+        <v>0.98920000000000008</v>
       </c>
     </row>
   </sheetData>
@@ -589,7 +559,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -601,7 +571,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>